<commit_message>
Handle sort product by range of price and view nearly out of stock product completed
</commit_message>
<xml_diff>
--- a/MyShopv2/importdata.xlsx
+++ b/MyShopv2/importdata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VuHiep\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VuHiep\source\repos\MyShopv2\MyShopv2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC462B7-6538-416B-9180-7EAF2F8E90B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756EE409-D728-44C3-822D-409417C36DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -905,8 +905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -966,7 +966,7 @@
         <v>114</v>
       </c>
       <c r="G4">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -1372,7 +1372,7 @@
         <v>128</v>
       </c>
       <c r="G18">
-        <v>660</v>
+        <v>2</v>
       </c>
       <c r="H18">
         <v>3</v>
@@ -1430,7 +1430,7 @@
         <v>130</v>
       </c>
       <c r="G20">
-        <v>1600</v>
+        <v>3</v>
       </c>
       <c r="H20">
         <v>4</v>
@@ -1575,7 +1575,7 @@
         <v>135</v>
       </c>
       <c r="G25">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="H25">
         <v>7</v>

</xml_diff>

<commit_message>
Add new product in product page
</commit_message>
<xml_diff>
--- a/MyShopv2/importdata.xlsx
+++ b/MyShopv2/importdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VuHiep\source\repos\MyShopv2\MyShopv2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756EE409-D728-44C3-822D-409417C36DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33352E61-3EBF-4EEA-95E6-4F1597B42AF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -905,8 +905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>